<commit_message>
atualizações % por linha
</commit_message>
<xml_diff>
--- a/Tabelas Censo 25-02-2025.xlsx
+++ b/Tabelas Censo 25-02-2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cesar_macieira\Desktop\Usiminas\Nescon\censo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE50B318-1F3E-4106-900F-5EAE0E8A3461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677005AC-FA56-4F24-9FAA-F5A243BA0A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-107" yWindow="-107" windowWidth="20847" windowHeight="11111" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -896,13 +896,19 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -917,15 +923,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -935,7 +932,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1236,7 +1236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:FH62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="EH1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1385,380 +1385,380 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:164" x14ac:dyDescent="0.3">
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
       <c r="V1" s="4"/>
-      <c r="X1" s="49" t="s">
+      <c r="X1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="49"/>
-      <c r="AB1" s="49" t="s">
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AB1" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="AC1" s="49"/>
-      <c r="AD1" s="49"/>
-      <c r="AF1" s="49" t="s">
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AF1" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="AG1" s="49"/>
-      <c r="AH1" s="49"/>
-      <c r="AI1" s="49"/>
-      <c r="AJ1" s="49"/>
-      <c r="AK1" s="49"/>
-      <c r="AL1" s="49"/>
-      <c r="AM1" s="49"/>
-      <c r="AN1" s="49"/>
-      <c r="AO1" s="49"/>
-      <c r="AP1" s="49"/>
-      <c r="AQ1" s="49"/>
-      <c r="AR1" s="49"/>
-      <c r="AS1" s="49"/>
-      <c r="AT1" s="49"/>
-      <c r="AU1" s="49"/>
-      <c r="AV1" s="49"/>
-      <c r="AW1" s="49"/>
-      <c r="AX1" s="49"/>
-      <c r="AY1" s="49"/>
+      <c r="AG1" s="50"/>
+      <c r="AH1" s="50"/>
+      <c r="AI1" s="50"/>
+      <c r="AJ1" s="50"/>
+      <c r="AK1" s="50"/>
+      <c r="AL1" s="50"/>
+      <c r="AM1" s="50"/>
+      <c r="AN1" s="50"/>
+      <c r="AO1" s="50"/>
+      <c r="AP1" s="50"/>
+      <c r="AQ1" s="50"/>
+      <c r="AR1" s="50"/>
+      <c r="AS1" s="50"/>
+      <c r="AT1" s="50"/>
+      <c r="AU1" s="50"/>
+      <c r="AV1" s="50"/>
+      <c r="AW1" s="50"/>
+      <c r="AX1" s="50"/>
+      <c r="AY1" s="50"/>
       <c r="AZ1" s="3"/>
-      <c r="BB1" s="49" t="s">
+      <c r="BB1" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="BC1" s="49"/>
-      <c r="BD1" s="49"/>
-      <c r="BE1" s="49"/>
-      <c r="BF1" s="49"/>
-      <c r="BG1" s="49"/>
-      <c r="BH1" s="49"/>
-      <c r="BI1" s="49"/>
-      <c r="BJ1" s="49"/>
-      <c r="BK1" s="49"/>
-      <c r="BL1" s="49"/>
-      <c r="BM1" s="49"/>
-      <c r="BN1" s="49"/>
-      <c r="BO1" s="49"/>
-      <c r="BP1" s="49"/>
-      <c r="BQ1" s="49"/>
-      <c r="BR1" s="49"/>
-      <c r="BS1" s="49"/>
-      <c r="BT1" s="49"/>
-      <c r="BU1" s="49"/>
+      <c r="BC1" s="50"/>
+      <c r="BD1" s="50"/>
+      <c r="BE1" s="50"/>
+      <c r="BF1" s="50"/>
+      <c r="BG1" s="50"/>
+      <c r="BH1" s="50"/>
+      <c r="BI1" s="50"/>
+      <c r="BJ1" s="50"/>
+      <c r="BK1" s="50"/>
+      <c r="BL1" s="50"/>
+      <c r="BM1" s="50"/>
+      <c r="BN1" s="50"/>
+      <c r="BO1" s="50"/>
+      <c r="BP1" s="50"/>
+      <c r="BQ1" s="50"/>
+      <c r="BR1" s="50"/>
+      <c r="BS1" s="50"/>
+      <c r="BT1" s="50"/>
+      <c r="BU1" s="50"/>
       <c r="BV1" s="3"/>
-      <c r="BX1" s="49" t="s">
+      <c r="BX1" s="50" t="s">
         <v>30</v>
       </c>
-      <c r="BY1" s="49"/>
-      <c r="BZ1" s="49"/>
-      <c r="CB1" s="49" t="s">
+      <c r="BY1" s="50"/>
+      <c r="BZ1" s="50"/>
+      <c r="CB1" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="CC1" s="49"/>
-      <c r="CD1" s="49"/>
-      <c r="CF1" s="49" t="s">
+      <c r="CC1" s="50"/>
+      <c r="CD1" s="50"/>
+      <c r="CF1" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="CG1" s="49"/>
-      <c r="CH1" s="49"/>
-      <c r="CJ1" s="49" t="s">
+      <c r="CG1" s="50"/>
+      <c r="CH1" s="50"/>
+      <c r="CJ1" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="CK1" s="49"/>
-      <c r="CL1" s="49"/>
-      <c r="CN1" s="49" t="s">
+      <c r="CK1" s="50"/>
+      <c r="CL1" s="50"/>
+      <c r="CN1" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="CO1" s="49"/>
-      <c r="CP1" s="49"/>
-      <c r="CR1" s="59" t="s">
+      <c r="CO1" s="50"/>
+      <c r="CP1" s="50"/>
+      <c r="CR1" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="CS1" s="59"/>
-      <c r="CT1" s="59"/>
-      <c r="CV1" s="59" t="s">
+      <c r="CS1" s="58"/>
+      <c r="CT1" s="58"/>
+      <c r="CV1" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="CW1" s="59"/>
-      <c r="CX1" s="59"/>
-      <c r="CZ1" s="49" t="s">
+      <c r="CW1" s="58"/>
+      <c r="CX1" s="58"/>
+      <c r="CZ1" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="DA1" s="49"/>
-      <c r="DB1" s="49"/>
-      <c r="DD1" s="49" t="s">
+      <c r="DA1" s="50"/>
+      <c r="DB1" s="50"/>
+      <c r="DD1" s="50" t="s">
         <v>74</v>
       </c>
-      <c r="DE1" s="49"/>
-      <c r="DF1" s="49"/>
-      <c r="DH1" s="49" t="s">
+      <c r="DE1" s="50"/>
+      <c r="DF1" s="50"/>
+      <c r="DH1" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="DI1" s="49"/>
-      <c r="DJ1" s="49"/>
-      <c r="DL1" s="49" t="s">
+      <c r="DI1" s="50"/>
+      <c r="DJ1" s="50"/>
+      <c r="DL1" s="50" t="s">
         <v>78</v>
       </c>
-      <c r="DM1" s="49"/>
-      <c r="DN1" s="49"/>
-      <c r="DP1" s="49" t="s">
+      <c r="DM1" s="50"/>
+      <c r="DN1" s="50"/>
+      <c r="DP1" s="50" t="s">
         <v>79</v>
       </c>
-      <c r="DQ1" s="49"/>
-      <c r="DR1" s="49"/>
-      <c r="DT1" s="49" t="s">
+      <c r="DQ1" s="50"/>
+      <c r="DR1" s="50"/>
+      <c r="DT1" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="DU1" s="49"/>
-      <c r="DV1" s="49"/>
-      <c r="DX1" s="49" t="s">
+      <c r="DU1" s="50"/>
+      <c r="DV1" s="50"/>
+      <c r="DX1" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="DY1" s="49"/>
-      <c r="DZ1" s="49"/>
+      <c r="DY1" s="50"/>
+      <c r="DZ1" s="50"/>
       <c r="EA1" s="3"/>
-      <c r="EB1" s="49" t="s">
+      <c r="EB1" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="EC1" s="49"/>
-      <c r="ED1" s="49"/>
-      <c r="EF1" s="49" t="s">
+      <c r="EC1" s="50"/>
+      <c r="ED1" s="50"/>
+      <c r="EF1" s="50" t="s">
         <v>179</v>
       </c>
-      <c r="EG1" s="49"/>
-      <c r="EH1" s="49"/>
-      <c r="EI1" s="49"/>
-      <c r="EJ1" s="49"/>
-      <c r="EK1" s="49"/>
-      <c r="EL1" s="49"/>
-      <c r="EM1" s="49"/>
-      <c r="EN1" s="49"/>
-      <c r="EO1" s="49"/>
-      <c r="EP1" s="49"/>
-      <c r="EQ1" s="49"/>
-      <c r="ER1" s="49"/>
-      <c r="ES1" s="49"/>
-      <c r="EU1" s="49" t="s">
+      <c r="EG1" s="50"/>
+      <c r="EH1" s="50"/>
+      <c r="EI1" s="50"/>
+      <c r="EJ1" s="50"/>
+      <c r="EK1" s="50"/>
+      <c r="EL1" s="50"/>
+      <c r="EM1" s="50"/>
+      <c r="EN1" s="50"/>
+      <c r="EO1" s="50"/>
+      <c r="EP1" s="50"/>
+      <c r="EQ1" s="50"/>
+      <c r="ER1" s="50"/>
+      <c r="ES1" s="50"/>
+      <c r="EU1" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="EV1" s="49"/>
-      <c r="EW1" s="49"/>
-      <c r="EX1" s="49"/>
-      <c r="EY1" s="49"/>
-      <c r="EZ1" s="49"/>
-      <c r="FA1" s="49"/>
-      <c r="FB1" s="49"/>
-      <c r="FC1" s="49"/>
-      <c r="FD1" s="49"/>
-      <c r="FE1" s="49"/>
-      <c r="FF1" s="49"/>
-      <c r="FG1" s="49"/>
-      <c r="FH1" s="49"/>
+      <c r="EV1" s="50"/>
+      <c r="EW1" s="50"/>
+      <c r="EX1" s="50"/>
+      <c r="EY1" s="50"/>
+      <c r="EZ1" s="50"/>
+      <c r="FA1" s="50"/>
+      <c r="FB1" s="50"/>
+      <c r="FC1" s="50"/>
+      <c r="FD1" s="50"/>
+      <c r="FE1" s="50"/>
+      <c r="FF1" s="50"/>
+      <c r="FG1" s="50"/>
+      <c r="FH1" s="50"/>
     </row>
     <row r="2" spans="2:164" x14ac:dyDescent="0.3">
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
       <c r="V2" s="4"/>
-      <c r="X2" s="50"/>
-      <c r="Y2" s="50"/>
-      <c r="Z2" s="50"/>
-      <c r="AB2" s="50"/>
-      <c r="AC2" s="50"/>
-      <c r="AD2" s="50"/>
-      <c r="AF2" s="50"/>
-      <c r="AG2" s="50"/>
-      <c r="AH2" s="50"/>
-      <c r="AI2" s="50"/>
-      <c r="AJ2" s="50"/>
-      <c r="AK2" s="50"/>
-      <c r="AL2" s="50"/>
-      <c r="AM2" s="50"/>
-      <c r="AN2" s="50"/>
-      <c r="AO2" s="50"/>
-      <c r="AP2" s="50"/>
-      <c r="AQ2" s="50"/>
-      <c r="AR2" s="50"/>
-      <c r="AS2" s="50"/>
-      <c r="AT2" s="50"/>
-      <c r="AU2" s="50"/>
-      <c r="AV2" s="50"/>
-      <c r="AW2" s="50"/>
-      <c r="AX2" s="50"/>
-      <c r="AY2" s="50"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="51"/>
+      <c r="AB2" s="51"/>
+      <c r="AC2" s="51"/>
+      <c r="AD2" s="51"/>
+      <c r="AF2" s="51"/>
+      <c r="AG2" s="51"/>
+      <c r="AH2" s="51"/>
+      <c r="AI2" s="51"/>
+      <c r="AJ2" s="51"/>
+      <c r="AK2" s="51"/>
+      <c r="AL2" s="51"/>
+      <c r="AM2" s="51"/>
+      <c r="AN2" s="51"/>
+      <c r="AO2" s="51"/>
+      <c r="AP2" s="51"/>
+      <c r="AQ2" s="51"/>
+      <c r="AR2" s="51"/>
+      <c r="AS2" s="51"/>
+      <c r="AT2" s="51"/>
+      <c r="AU2" s="51"/>
+      <c r="AV2" s="51"/>
+      <c r="AW2" s="51"/>
+      <c r="AX2" s="51"/>
+      <c r="AY2" s="51"/>
       <c r="AZ2" s="3"/>
-      <c r="BB2" s="50"/>
-      <c r="BC2" s="50"/>
-      <c r="BD2" s="50"/>
-      <c r="BE2" s="50"/>
-      <c r="BF2" s="50"/>
-      <c r="BG2" s="50"/>
-      <c r="BH2" s="50"/>
-      <c r="BI2" s="50"/>
-      <c r="BJ2" s="50"/>
-      <c r="BK2" s="50"/>
-      <c r="BL2" s="50"/>
-      <c r="BM2" s="50"/>
-      <c r="BN2" s="50"/>
-      <c r="BO2" s="50"/>
-      <c r="BP2" s="50"/>
-      <c r="BQ2" s="50"/>
-      <c r="BR2" s="50"/>
-      <c r="BS2" s="50"/>
-      <c r="BT2" s="50"/>
-      <c r="BU2" s="50"/>
+      <c r="BB2" s="51"/>
+      <c r="BC2" s="51"/>
+      <c r="BD2" s="51"/>
+      <c r="BE2" s="51"/>
+      <c r="BF2" s="51"/>
+      <c r="BG2" s="51"/>
+      <c r="BH2" s="51"/>
+      <c r="BI2" s="51"/>
+      <c r="BJ2" s="51"/>
+      <c r="BK2" s="51"/>
+      <c r="BL2" s="51"/>
+      <c r="BM2" s="51"/>
+      <c r="BN2" s="51"/>
+      <c r="BO2" s="51"/>
+      <c r="BP2" s="51"/>
+      <c r="BQ2" s="51"/>
+      <c r="BR2" s="51"/>
+      <c r="BS2" s="51"/>
+      <c r="BT2" s="51"/>
+      <c r="BU2" s="51"/>
       <c r="BV2" s="3"/>
-      <c r="BX2" s="49"/>
-      <c r="BY2" s="49"/>
-      <c r="BZ2" s="49"/>
-      <c r="CB2" s="49"/>
-      <c r="CC2" s="49"/>
-      <c r="CD2" s="49"/>
-      <c r="CF2" s="49"/>
-      <c r="CG2" s="49"/>
-      <c r="CH2" s="49"/>
-      <c r="CJ2" s="49"/>
-      <c r="CK2" s="49"/>
-      <c r="CL2" s="49"/>
-      <c r="CN2" s="49"/>
-      <c r="CO2" s="49"/>
-      <c r="CP2" s="49"/>
-      <c r="CR2" s="59"/>
-      <c r="CS2" s="59"/>
-      <c r="CT2" s="59"/>
-      <c r="CV2" s="59"/>
-      <c r="CW2" s="59"/>
-      <c r="CX2" s="59"/>
-      <c r="CZ2" s="49"/>
-      <c r="DA2" s="49"/>
-      <c r="DB2" s="49"/>
-      <c r="DD2" s="49"/>
-      <c r="DE2" s="49"/>
-      <c r="DF2" s="49"/>
-      <c r="DH2" s="49"/>
-      <c r="DI2" s="49"/>
-      <c r="DJ2" s="49"/>
-      <c r="DL2" s="49"/>
-      <c r="DM2" s="49"/>
-      <c r="DN2" s="49"/>
-      <c r="DP2" s="49"/>
-      <c r="DQ2" s="49"/>
-      <c r="DR2" s="49"/>
-      <c r="DT2" s="49"/>
-      <c r="DU2" s="49"/>
-      <c r="DV2" s="49"/>
-      <c r="DX2" s="49"/>
-      <c r="DY2" s="49"/>
-      <c r="DZ2" s="49"/>
+      <c r="BX2" s="50"/>
+      <c r="BY2" s="50"/>
+      <c r="BZ2" s="50"/>
+      <c r="CB2" s="50"/>
+      <c r="CC2" s="50"/>
+      <c r="CD2" s="50"/>
+      <c r="CF2" s="50"/>
+      <c r="CG2" s="50"/>
+      <c r="CH2" s="50"/>
+      <c r="CJ2" s="50"/>
+      <c r="CK2" s="50"/>
+      <c r="CL2" s="50"/>
+      <c r="CN2" s="50"/>
+      <c r="CO2" s="50"/>
+      <c r="CP2" s="50"/>
+      <c r="CR2" s="58"/>
+      <c r="CS2" s="58"/>
+      <c r="CT2" s="58"/>
+      <c r="CV2" s="58"/>
+      <c r="CW2" s="58"/>
+      <c r="CX2" s="58"/>
+      <c r="CZ2" s="50"/>
+      <c r="DA2" s="50"/>
+      <c r="DB2" s="50"/>
+      <c r="DD2" s="50"/>
+      <c r="DE2" s="50"/>
+      <c r="DF2" s="50"/>
+      <c r="DH2" s="50"/>
+      <c r="DI2" s="50"/>
+      <c r="DJ2" s="50"/>
+      <c r="DL2" s="50"/>
+      <c r="DM2" s="50"/>
+      <c r="DN2" s="50"/>
+      <c r="DP2" s="50"/>
+      <c r="DQ2" s="50"/>
+      <c r="DR2" s="50"/>
+      <c r="DT2" s="50"/>
+      <c r="DU2" s="50"/>
+      <c r="DV2" s="50"/>
+      <c r="DX2" s="50"/>
+      <c r="DY2" s="50"/>
+      <c r="DZ2" s="50"/>
       <c r="EA2" s="3"/>
-      <c r="EB2" s="49"/>
-      <c r="EC2" s="49"/>
-      <c r="ED2" s="49"/>
-      <c r="EF2" s="50"/>
-      <c r="EG2" s="50"/>
-      <c r="EH2" s="50"/>
-      <c r="EI2" s="50"/>
-      <c r="EJ2" s="50"/>
-      <c r="EK2" s="50"/>
-      <c r="EL2" s="50"/>
-      <c r="EM2" s="50"/>
-      <c r="EN2" s="50"/>
-      <c r="EO2" s="50"/>
-      <c r="EP2" s="50"/>
-      <c r="EQ2" s="50"/>
-      <c r="ER2" s="50"/>
-      <c r="ES2" s="50"/>
-      <c r="EU2" s="50"/>
-      <c r="EV2" s="50"/>
-      <c r="EW2" s="50"/>
-      <c r="EX2" s="50"/>
-      <c r="EY2" s="50"/>
-      <c r="EZ2" s="50"/>
-      <c r="FA2" s="50"/>
-      <c r="FB2" s="50"/>
-      <c r="FC2" s="50"/>
-      <c r="FD2" s="50"/>
-      <c r="FE2" s="50"/>
-      <c r="FF2" s="50"/>
-      <c r="FG2" s="50"/>
-      <c r="FH2" s="50"/>
+      <c r="EB2" s="50"/>
+      <c r="EC2" s="50"/>
+      <c r="ED2" s="50"/>
+      <c r="EF2" s="51"/>
+      <c r="EG2" s="51"/>
+      <c r="EH2" s="51"/>
+      <c r="EI2" s="51"/>
+      <c r="EJ2" s="51"/>
+      <c r="EK2" s="51"/>
+      <c r="EL2" s="51"/>
+      <c r="EM2" s="51"/>
+      <c r="EN2" s="51"/>
+      <c r="EO2" s="51"/>
+      <c r="EP2" s="51"/>
+      <c r="EQ2" s="51"/>
+      <c r="ER2" s="51"/>
+      <c r="ES2" s="51"/>
+      <c r="EU2" s="51"/>
+      <c r="EV2" s="51"/>
+      <c r="EW2" s="51"/>
+      <c r="EX2" s="51"/>
+      <c r="EY2" s="51"/>
+      <c r="EZ2" s="51"/>
+      <c r="FA2" s="51"/>
+      <c r="FB2" s="51"/>
+      <c r="FC2" s="51"/>
+      <c r="FD2" s="51"/>
+      <c r="FE2" s="51"/>
+      <c r="FF2" s="51"/>
+      <c r="FG2" s="51"/>
+      <c r="FH2" s="51"/>
     </row>
     <row r="3" spans="2:164" x14ac:dyDescent="0.3">
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="53" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51">
+      <c r="C3" s="53"/>
+      <c r="D3" s="53">
         <v>0</v>
       </c>
-      <c r="E3" s="51"/>
-      <c r="F3" s="54">
+      <c r="E3" s="53"/>
+      <c r="F3" s="56">
         <v>1</v>
       </c>
-      <c r="G3" s="53"/>
-      <c r="H3" s="51">
+      <c r="G3" s="55"/>
+      <c r="H3" s="53">
         <v>2</v>
       </c>
-      <c r="I3" s="51"/>
-      <c r="J3" s="54">
+      <c r="I3" s="53"/>
+      <c r="J3" s="56">
         <v>3</v>
       </c>
-      <c r="K3" s="53"/>
-      <c r="L3" s="51">
+      <c r="K3" s="55"/>
+      <c r="L3" s="53">
         <v>4</v>
       </c>
-      <c r="M3" s="51"/>
-      <c r="N3" s="54">
+      <c r="M3" s="53"/>
+      <c r="N3" s="56">
         <v>5</v>
       </c>
-      <c r="O3" s="53"/>
-      <c r="P3" s="54">
+      <c r="O3" s="55"/>
+      <c r="P3" s="56">
         <v>6</v>
       </c>
-      <c r="Q3" s="53"/>
-      <c r="R3" s="51" t="s">
+      <c r="Q3" s="55"/>
+      <c r="R3" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="S3" s="51"/>
-      <c r="T3" s="56" t="s">
+      <c r="S3" s="53"/>
+      <c r="T3" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="51" t="s">
+      <c r="U3" s="53" t="s">
         <v>12</v>
       </c>
       <c r="V3" s="36"/>
@@ -1780,89 +1780,89 @@
       <c r="AD3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="AF3" s="51" t="s">
+      <c r="AF3" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="AG3" s="51"/>
-      <c r="AH3" s="51">
+      <c r="AG3" s="53"/>
+      <c r="AH3" s="53">
         <v>0</v>
       </c>
-      <c r="AI3" s="51"/>
-      <c r="AJ3" s="54">
+      <c r="AI3" s="53"/>
+      <c r="AJ3" s="56">
         <v>1</v>
       </c>
-      <c r="AK3" s="53"/>
-      <c r="AL3" s="51">
+      <c r="AK3" s="55"/>
+      <c r="AL3" s="53">
         <v>2</v>
       </c>
-      <c r="AM3" s="51"/>
-      <c r="AN3" s="54">
+      <c r="AM3" s="53"/>
+      <c r="AN3" s="56">
         <v>3</v>
       </c>
-      <c r="AO3" s="53"/>
-      <c r="AP3" s="51">
+      <c r="AO3" s="55"/>
+      <c r="AP3" s="53">
         <v>4</v>
       </c>
-      <c r="AQ3" s="51"/>
-      <c r="AR3" s="54">
+      <c r="AQ3" s="53"/>
+      <c r="AR3" s="56">
         <v>5</v>
       </c>
-      <c r="AS3" s="53"/>
-      <c r="AT3" s="54">
+      <c r="AS3" s="55"/>
+      <c r="AT3" s="56">
         <v>6</v>
       </c>
-      <c r="AU3" s="53"/>
-      <c r="AV3" s="51" t="s">
+      <c r="AU3" s="55"/>
+      <c r="AV3" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="AW3" s="51"/>
-      <c r="AX3" s="56" t="s">
+      <c r="AW3" s="53"/>
+      <c r="AX3" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="AY3" s="51" t="s">
+      <c r="AY3" s="53" t="s">
         <v>12</v>
       </c>
       <c r="AZ3" s="35"/>
-      <c r="BB3" s="51" t="s">
+      <c r="BB3" s="53" t="s">
         <v>22</v>
       </c>
-      <c r="BC3" s="51"/>
-      <c r="BD3" s="51" t="s">
+      <c r="BC3" s="53"/>
+      <c r="BD3" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="BE3" s="51"/>
-      <c r="BF3" s="54" t="s">
+      <c r="BE3" s="53"/>
+      <c r="BF3" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="BG3" s="53"/>
-      <c r="BH3" s="51" t="s">
+      <c r="BG3" s="55"/>
+      <c r="BH3" s="53" t="s">
         <v>33</v>
       </c>
-      <c r="BI3" s="51"/>
-      <c r="BJ3" s="54" t="s">
+      <c r="BI3" s="53"/>
+      <c r="BJ3" s="56" t="s">
         <v>34</v>
       </c>
-      <c r="BK3" s="53"/>
-      <c r="BL3" s="51" t="s">
+      <c r="BK3" s="55"/>
+      <c r="BL3" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="BM3" s="51"/>
-      <c r="BN3" s="54" t="s">
+      <c r="BM3" s="53"/>
+      <c r="BN3" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="BO3" s="53"/>
-      <c r="BP3" s="54" t="s">
+      <c r="BO3" s="55"/>
+      <c r="BP3" s="56" t="s">
         <v>37</v>
       </c>
-      <c r="BQ3" s="53"/>
-      <c r="BR3" s="51" t="s">
+      <c r="BQ3" s="55"/>
+      <c r="BR3" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="BS3" s="51"/>
-      <c r="BT3" s="56" t="s">
+      <c r="BS3" s="53"/>
+      <c r="BT3" s="60" t="s">
         <v>7</v>
       </c>
-      <c r="BU3" s="51" t="s">
+      <c r="BU3" s="53" t="s">
         <v>12</v>
       </c>
       <c r="BV3" s="35"/>
@@ -2002,70 +2002,70 @@
       <c r="ED3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="EF3" s="51" t="s">
+      <c r="EF3" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="EG3" s="51" t="s">
+      <c r="EG3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="EH3" s="53"/>
-      <c r="EI3" s="51" t="s">
+      <c r="EH3" s="55"/>
+      <c r="EI3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="EJ3" s="53"/>
-      <c r="EK3" s="54" t="s">
+      <c r="EJ3" s="55"/>
+      <c r="EK3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="EL3" s="53"/>
-      <c r="EM3" s="51" t="s">
+      <c r="EL3" s="55"/>
+      <c r="EM3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="EN3" s="53"/>
-      <c r="EO3" s="51" t="s">
+      <c r="EN3" s="55"/>
+      <c r="EO3" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="EP3" s="51"/>
-      <c r="EQ3" s="51" t="s">
+      <c r="EP3" s="53"/>
+      <c r="EQ3" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="ER3" s="55" t="s">
+      <c r="ER3" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="ES3" s="55"/>
-      <c r="EU3" s="51" t="s">
+      <c r="ES3" s="49"/>
+      <c r="EU3" s="53" t="s">
         <v>150</v>
       </c>
-      <c r="EV3" s="51" t="s">
+      <c r="EV3" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="EW3" s="53"/>
-      <c r="EX3" s="51" t="s">
+      <c r="EW3" s="55"/>
+      <c r="EX3" s="53" t="s">
         <v>3</v>
       </c>
-      <c r="EY3" s="53"/>
-      <c r="EZ3" s="54" t="s">
+      <c r="EY3" s="55"/>
+      <c r="EZ3" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="FA3" s="53"/>
-      <c r="FB3" s="51" t="s">
+      <c r="FA3" s="55"/>
+      <c r="FB3" s="53" t="s">
         <v>5</v>
       </c>
-      <c r="FC3" s="53"/>
-      <c r="FD3" s="51" t="s">
+      <c r="FC3" s="55"/>
+      <c r="FD3" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="FE3" s="51"/>
-      <c r="FF3" s="51" t="s">
+      <c r="FE3" s="53"/>
+      <c r="FF3" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="FG3" s="55" t="s">
+      <c r="FG3" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="FH3" s="55"/>
+      <c r="FH3" s="49"/>
     </row>
     <row r="4" spans="2:164" x14ac:dyDescent="0.3">
-      <c r="B4" s="52"/>
-      <c r="C4" s="52"/>
+      <c r="B4" s="54"/>
+      <c r="C4" s="54"/>
       <c r="D4" s="5" t="s">
         <v>0</v>
       </c>
@@ -2114,8 +2114,8 @@
       <c r="S4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="T4" s="57"/>
-      <c r="U4" s="52"/>
+      <c r="T4" s="61"/>
+      <c r="U4" s="54"/>
       <c r="V4" s="36"/>
       <c r="X4" s="9" t="s">
         <v>16</v>
@@ -2135,8 +2135,8 @@
       <c r="AD4" s="23">
         <v>0.75167590922251204</v>
       </c>
-      <c r="AF4" s="52"/>
-      <c r="AG4" s="52"/>
+      <c r="AF4" s="54"/>
+      <c r="AG4" s="54"/>
       <c r="AH4" s="5" t="s">
         <v>0</v>
       </c>
@@ -2185,11 +2185,11 @@
       <c r="AW4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="AX4" s="57"/>
-      <c r="AY4" s="52"/>
+      <c r="AX4" s="61"/>
+      <c r="AY4" s="54"/>
       <c r="AZ4" s="35"/>
-      <c r="BB4" s="52"/>
-      <c r="BC4" s="52"/>
+      <c r="BB4" s="54"/>
+      <c r="BC4" s="54"/>
       <c r="BD4" s="5" t="s">
         <v>0</v>
       </c>
@@ -2238,8 +2238,8 @@
       <c r="BS4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="BT4" s="57"/>
-      <c r="BU4" s="52"/>
+      <c r="BT4" s="61"/>
+      <c r="BU4" s="54"/>
       <c r="BV4" s="35"/>
       <c r="BX4" s="9" t="s">
         <v>28</v>
@@ -2376,7 +2376,7 @@
       <c r="ED4" s="11">
         <v>3.4381467387676098E-2</v>
       </c>
-      <c r="EF4" s="52"/>
+      <c r="EF4" s="54"/>
       <c r="EG4" s="5" t="s">
         <v>0</v>
       </c>
@@ -2407,14 +2407,14 @@
       <c r="EP4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="EQ4" s="52"/>
+      <c r="EQ4" s="54"/>
       <c r="ER4" s="5" t="s">
         <v>0</v>
       </c>
       <c r="ES4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="EU4" s="52"/>
+      <c r="EU4" s="54"/>
       <c r="EV4" s="5" t="s">
         <v>0</v>
       </c>
@@ -2445,7 +2445,7 @@
       <c r="FE4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="FF4" s="52"/>
+      <c r="FF4" s="54"/>
       <c r="FG4" s="5" t="s">
         <v>0</v>
       </c>
@@ -2454,7 +2454,7 @@
       </c>
     </row>
     <row r="5" spans="2:164" ht="14" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="58" t="s">
+      <c r="B5" s="57" t="s">
         <v>15</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -2508,7 +2508,7 @@
       <c r="S5" s="11">
         <v>0.58051529790660195</v>
       </c>
-      <c r="T5" s="48" t="s">
+      <c r="T5" s="52" t="s">
         <v>8</v>
       </c>
       <c r="U5" s="10">
@@ -2537,7 +2537,7 @@
       <c r="AD5" s="24">
         <v>0.24832409077748799</v>
       </c>
-      <c r="AF5" s="58" t="s">
+      <c r="AF5" s="57" t="s">
         <v>23</v>
       </c>
       <c r="AG5" s="9" t="s">
@@ -2591,7 +2591,7 @@
       <c r="AW5" s="11">
         <v>0.59107142857142903</v>
       </c>
-      <c r="AX5" s="48" t="s">
+      <c r="AX5" s="52" t="s">
         <v>8</v>
       </c>
       <c r="AY5" s="10">
@@ -2602,7 +2602,7 @@
         <f>AY5/AY10</f>
         <v>0.50755973190229131</v>
       </c>
-      <c r="BB5" s="58" t="s">
+      <c r="BB5" s="57" t="s">
         <v>23</v>
       </c>
       <c r="BC5" s="9" t="s">
@@ -2656,7 +2656,7 @@
       <c r="BS5" s="11">
         <v>0.59107142857142903</v>
       </c>
-      <c r="BT5" s="48" t="s">
+      <c r="BT5" s="52" t="s">
         <v>8</v>
       </c>
       <c r="BU5" s="10">
@@ -2835,7 +2835,7 @@
       <c r="EP5" s="23">
         <v>3.0894308943089401E-2</v>
       </c>
-      <c r="EQ5" s="48" t="s">
+      <c r="EQ5" s="52" t="s">
         <v>8</v>
       </c>
       <c r="ER5" s="3">
@@ -2879,7 +2879,7 @@
       <c r="FE5" s="23">
         <v>9.27734375E-3</v>
       </c>
-      <c r="FF5" s="48" t="s">
+      <c r="FF5" s="52" t="s">
         <v>8</v>
       </c>
       <c r="FG5" s="3">
@@ -2892,7 +2892,7 @@
       </c>
     </row>
     <row r="6" spans="2:164" x14ac:dyDescent="0.3">
-      <c r="B6" s="59"/>
+      <c r="B6" s="58"/>
       <c r="C6" t="s">
         <v>3</v>
       </c>
@@ -2944,7 +2944,7 @@
       <c r="S6" s="4">
         <v>0.16505636070853499</v>
       </c>
-      <c r="T6" s="49"/>
+      <c r="T6" s="50"/>
       <c r="U6" s="3">
         <f t="shared" ref="U6:U9" si="0">SUM(D6,F6,H6,J6,L6,N6,P6,R6)</f>
         <v>12280</v>
@@ -2975,7 +2975,7 @@
         <f>SUM(AD4:AD5)</f>
         <v>1</v>
       </c>
-      <c r="AF6" s="59"/>
+      <c r="AF6" s="58"/>
       <c r="AG6" t="s">
         <v>3</v>
       </c>
@@ -3027,7 +3027,7 @@
       <c r="AW6" s="4">
         <v>5.7142857142857099E-2</v>
       </c>
-      <c r="AX6" s="49"/>
+      <c r="AX6" s="50"/>
       <c r="AY6" s="3">
         <f>SUM(AH6,AJ6,AL6,AN6,AP6,AR6,AT6,AV6)</f>
         <v>2533</v>
@@ -3036,7 +3036,7 @@
         <f>AY6/AY10</f>
         <v>5.6402948184105635E-2</v>
       </c>
-      <c r="BB6" s="59"/>
+      <c r="BB6" s="58"/>
       <c r="BC6" t="s">
         <v>3</v>
       </c>
@@ -3088,7 +3088,7 @@
       <c r="BS6" s="4">
         <v>5.7142857142857099E-2</v>
       </c>
-      <c r="BT6" s="49"/>
+      <c r="BT6" s="50"/>
       <c r="BU6" s="3">
         <f>SUM(BD6,BF6,BH6,BJ6,BL6,BN6,BP6,BR6)</f>
         <v>2533</v>
@@ -3271,7 +3271,7 @@
       <c r="EP6" s="2">
         <v>7.8048780487804906E-2</v>
       </c>
-      <c r="EQ6" s="49"/>
+      <c r="EQ6" s="50"/>
       <c r="ER6" s="3">
         <f t="shared" ref="ER6:ER37" si="1">SUM(EG6,EI6,EK6,EM6,EO6)</f>
         <v>17737</v>
@@ -3313,7 +3313,7 @@
       <c r="FE6" s="2">
         <v>5.4124147262784002E-3</v>
       </c>
-      <c r="FF6" s="49"/>
+      <c r="FF6" s="50"/>
       <c r="FG6" s="3">
         <f t="shared" ref="FG6:FG10" si="2">SUM(EV6,EX6,EZ6,FB6,FD6)</f>
         <v>17737</v>
@@ -3324,7 +3324,7 @@
       </c>
     </row>
     <row r="7" spans="2:164" x14ac:dyDescent="0.3">
-      <c r="B7" s="59"/>
+      <c r="B7" s="58"/>
       <c r="C7" t="s">
         <v>4</v>
       </c>
@@ -3376,7 +3376,7 @@
       <c r="S7" s="4">
         <v>8.0515297906602196E-3</v>
       </c>
-      <c r="T7" s="49"/>
+      <c r="T7" s="50"/>
       <c r="U7" s="3">
         <f t="shared" si="0"/>
         <v>11020</v>
@@ -3385,7 +3385,7 @@
         <f>U7/U10</f>
         <v>0.24531956100710137</v>
       </c>
-      <c r="AF7" s="59"/>
+      <c r="AF7" s="58"/>
       <c r="AG7" t="s">
         <v>4</v>
       </c>
@@ -3437,7 +3437,7 @@
       <c r="AW7" s="4">
         <v>5.3571428571428598E-3</v>
       </c>
-      <c r="AX7" s="49"/>
+      <c r="AX7" s="50"/>
       <c r="AY7" s="3">
         <f>SUM(AH7,AJ7,AL7,AN7,AP7,AR7,AT7,AV7)</f>
         <v>1411</v>
@@ -3446,7 +3446,7 @@
         <f>AY7/AY10</f>
         <v>3.141909194148166E-2</v>
       </c>
-      <c r="BB7" s="59"/>
+      <c r="BB7" s="58"/>
       <c r="BC7" t="s">
         <v>4</v>
       </c>
@@ -3498,7 +3498,7 @@
       <c r="BS7" s="4">
         <v>5.3571428571428598E-3</v>
       </c>
-      <c r="BT7" s="49"/>
+      <c r="BT7" s="50"/>
       <c r="BU7" s="3">
         <f>SUM(BD7,BF7,BH7,BJ7,BL7,BN7,BP7,BR7)</f>
         <v>1411</v>
@@ -3652,7 +3652,7 @@
       <c r="EP7" s="2">
         <v>0.38780487804878</v>
       </c>
-      <c r="EQ7" s="49"/>
+      <c r="EQ7" s="50"/>
       <c r="ER7" s="3">
         <f t="shared" si="1"/>
         <v>13374</v>
@@ -3694,7 +3694,7 @@
       <c r="FE7" s="2">
         <v>3.5666218034993299E-2</v>
       </c>
-      <c r="FF7" s="49"/>
+      <c r="FF7" s="50"/>
       <c r="FG7" s="3">
         <f t="shared" si="2"/>
         <v>13374</v>
@@ -3705,7 +3705,7 @@
       </c>
     </row>
     <row r="8" spans="2:164" x14ac:dyDescent="0.3">
-      <c r="B8" s="59"/>
+      <c r="B8" s="58"/>
       <c r="C8" t="s">
         <v>5</v>
       </c>
@@ -3757,7 +3757,7 @@
       <c r="S8" s="4">
         <v>0.15942028985507201</v>
       </c>
-      <c r="T8" s="49"/>
+      <c r="T8" s="50"/>
       <c r="U8" s="3">
         <f t="shared" si="0"/>
         <v>6415</v>
@@ -3766,7 +3766,7 @@
         <f>U8/U10</f>
         <v>0.14280625987845327</v>
       </c>
-      <c r="AF8" s="59"/>
+      <c r="AF8" s="58"/>
       <c r="AG8" t="s">
         <v>5</v>
       </c>
@@ -3818,7 +3818,7 @@
       <c r="AW8" s="4">
         <v>2.6785714285714302E-2</v>
       </c>
-      <c r="AX8" s="49"/>
+      <c r="AX8" s="50"/>
       <c r="AY8" s="3">
         <f>SUM(AH8,AJ8,AL8,AN8,AP8,AR8,AT8,AV8)</f>
         <v>2203</v>
@@ -3827,7 +3827,7 @@
         <f>AY8/AY10</f>
         <v>4.9054755171569174E-2</v>
       </c>
-      <c r="BB8" s="59"/>
+      <c r="BB8" s="58"/>
       <c r="BC8" t="s">
         <v>5</v>
       </c>
@@ -3879,7 +3879,7 @@
       <c r="BS8" s="4">
         <v>2.6785714285714302E-2</v>
       </c>
-      <c r="BT8" s="49"/>
+      <c r="BT8" s="50"/>
       <c r="BU8" s="3">
         <f>SUM(BD8,BF8,BH8,BJ8,BL8,BN8,BP8,BR8)</f>
         <v>2203</v>
@@ -3955,11 +3955,11 @@
         <f>SUM(DJ4:DJ7)</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="DL8" s="61" t="s">
+      <c r="DL8" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="DM8" s="61"/>
-      <c r="DN8" s="61"/>
+      <c r="DM8" s="48"/>
+      <c r="DN8" s="48"/>
       <c r="DP8" s="12" t="s">
         <v>6</v>
       </c>
@@ -4020,7 +4020,7 @@
       <c r="EP8" s="2">
         <v>0.45365853658536598</v>
       </c>
-      <c r="EQ8" s="49"/>
+      <c r="EQ8" s="50"/>
       <c r="ER8" s="3">
         <f t="shared" si="1"/>
         <v>6607</v>
@@ -4062,7 +4062,7 @@
       <c r="FE8" s="2">
         <v>8.4455880127137894E-2</v>
       </c>
-      <c r="FF8" s="49"/>
+      <c r="FF8" s="50"/>
       <c r="FG8" s="3">
         <f t="shared" si="2"/>
         <v>6607</v>
@@ -4073,7 +4073,7 @@
       </c>
     </row>
     <row r="9" spans="2:164" x14ac:dyDescent="0.3">
-      <c r="B9" s="60"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="12" t="s">
         <v>6</v>
       </c>
@@ -4125,7 +4125,7 @@
       <c r="S9" s="14">
         <v>8.6956521739130405E-2</v>
       </c>
-      <c r="T9" s="50"/>
+      <c r="T9" s="51"/>
       <c r="U9" s="13">
         <f t="shared" si="0"/>
         <v>5272</v>
@@ -4134,7 +4134,7 @@
         <f>U9/U10</f>
         <v>0.11736159034749895</v>
       </c>
-      <c r="AF9" s="60"/>
+      <c r="AF9" s="59"/>
       <c r="AG9" s="12" t="s">
         <v>6</v>
       </c>
@@ -4186,7 +4186,7 @@
       <c r="AW9" s="14">
         <v>0.31964285714285701</v>
       </c>
-      <c r="AX9" s="50"/>
+      <c r="AX9" s="51"/>
       <c r="AY9" s="13">
         <f>SUM(AH9,AJ9,AL9,AN9,AP9,AR9,AT9,AV9)</f>
         <v>15968</v>
@@ -4195,7 +4195,7 @@
         <f>AY9/AY10</f>
         <v>0.35556347280055223</v>
       </c>
-      <c r="BB9" s="60"/>
+      <c r="BB9" s="59"/>
       <c r="BC9" s="12" t="s">
         <v>6</v>
       </c>
@@ -4247,7 +4247,7 @@
       <c r="BS9" s="14">
         <v>0.31964285714285701</v>
       </c>
-      <c r="BT9" s="50"/>
+      <c r="BT9" s="51"/>
       <c r="BU9" s="13">
         <f>SUM(BD9,BF9,BH9,BJ9,BL9,BN9,BP9,BR9)</f>
         <v>15968</v>
@@ -4307,9 +4307,9 @@
         <f>SUM(DF4:DF8)</f>
         <v>1</v>
       </c>
-      <c r="DL9" s="61"/>
-      <c r="DM9" s="61"/>
-      <c r="DN9" s="61"/>
+      <c r="DL9" s="48"/>
+      <c r="DM9" s="48"/>
+      <c r="DN9" s="48"/>
       <c r="DP9" s="25" t="s">
         <v>12</v>
       </c>
@@ -4374,7 +4374,7 @@
       <c r="EP9" s="24">
         <v>4.9593495934959299E-2</v>
       </c>
-      <c r="EQ9" s="50"/>
+      <c r="EQ9" s="51"/>
       <c r="ER9" s="3">
         <f t="shared" si="1"/>
         <v>3123</v>
@@ -4416,7 +4416,7 @@
       <c r="FE9" s="24">
         <v>1.95325008005123E-2</v>
       </c>
-      <c r="FF9" s="50"/>
+      <c r="FF9" s="51"/>
       <c r="FG9" s="3">
         <f t="shared" si="2"/>
         <v>3123</v>
@@ -4612,11 +4612,11 @@
     </row>
     <row r="11" spans="2:164" x14ac:dyDescent="0.3">
       <c r="BU11" s="3"/>
-      <c r="CB11" s="61" t="s">
+      <c r="CB11" s="48" t="s">
         <v>181</v>
       </c>
-      <c r="CC11" s="61"/>
-      <c r="CD11" s="61"/>
+      <c r="CC11" s="48"/>
+      <c r="CD11" s="48"/>
       <c r="CR11" t="s">
         <v>54</v>
       </c>
@@ -4635,16 +4635,16 @@
       <c r="CX11" s="2">
         <v>1.9516211585107999E-2</v>
       </c>
-      <c r="CZ11" s="61" t="s">
+      <c r="CZ11" s="48" t="s">
         <v>182</v>
       </c>
-      <c r="DA11" s="61"/>
-      <c r="DB11" s="61"/>
-      <c r="DD11" s="61" t="s">
+      <c r="DA11" s="48"/>
+      <c r="DB11" s="48"/>
+      <c r="DD11" s="48" t="s">
         <v>184</v>
       </c>
-      <c r="DE11" s="61"/>
-      <c r="DF11" s="61"/>
+      <c r="DE11" s="48"/>
+      <c r="DF11" s="48"/>
       <c r="DL11" s="9" t="s">
         <v>41</v>
       </c>
@@ -4696,7 +4696,7 @@
       <c r="EP11" s="23">
         <v>0</v>
       </c>
-      <c r="EQ11" s="48" t="s">
+      <c r="EQ11" s="52" t="s">
         <v>8</v>
       </c>
       <c r="ER11" s="3">
@@ -4740,7 +4740,7 @@
       <c r="FE11" s="23">
         <v>0</v>
       </c>
-      <c r="FF11" s="48" t="s">
+      <c r="FF11" s="52" t="s">
         <v>8</v>
       </c>
       <c r="FG11" s="3">
@@ -4753,9 +4753,9 @@
       </c>
     </row>
     <row r="12" spans="2:164" x14ac:dyDescent="0.3">
-      <c r="CB12" s="61"/>
-      <c r="CC12" s="61"/>
-      <c r="CD12" s="61"/>
+      <c r="CB12" s="48"/>
+      <c r="CC12" s="48"/>
+      <c r="CD12" s="48"/>
       <c r="CR12" s="9" t="s">
         <v>55</v>
       </c>
@@ -4774,12 +4774,12 @@
       <c r="CX12" s="2">
         <v>9.8359926118788497E-3</v>
       </c>
-      <c r="CZ12" s="61"/>
-      <c r="DA12" s="61"/>
-      <c r="DB12" s="61"/>
-      <c r="DD12" s="61"/>
-      <c r="DE12" s="61"/>
-      <c r="DF12" s="61"/>
+      <c r="CZ12" s="48"/>
+      <c r="DA12" s="48"/>
+      <c r="DB12" s="48"/>
+      <c r="DD12" s="48"/>
+      <c r="DE12" s="48"/>
+      <c r="DF12" s="48"/>
       <c r="DL12" s="12" t="s">
         <v>42</v>
       </c>
@@ -4831,7 +4831,7 @@
       <c r="EP12" s="2">
         <v>0</v>
       </c>
-      <c r="EQ12" s="49"/>
+      <c r="EQ12" s="50"/>
       <c r="ER12" s="3">
         <f t="shared" si="1"/>
         <v>996</v>
@@ -4873,7 +4873,7 @@
       <c r="FE12" s="2">
         <v>0</v>
       </c>
-      <c r="FF12" s="49"/>
+      <c r="FF12" s="50"/>
       <c r="FG12" s="3">
         <f t="shared" ref="FG12:FG38" si="7">SUM(EV12,EX12,EZ12,FB12,FD12)</f>
         <v>996</v>
@@ -4982,7 +4982,7 @@
       <c r="EP13" s="2">
         <v>2.4390243902438998E-3</v>
       </c>
-      <c r="EQ13" s="49"/>
+      <c r="EQ13" s="50"/>
       <c r="ER13" s="3">
         <f t="shared" si="1"/>
         <v>656</v>
@@ -5024,7 +5024,7 @@
       <c r="FE13" s="2">
         <v>4.5731707317073203E-3</v>
       </c>
-      <c r="FF13" s="49"/>
+      <c r="FF13" s="50"/>
       <c r="FG13" s="3">
         <f t="shared" si="7"/>
         <v>656</v>
@@ -5122,7 +5122,7 @@
       <c r="EP14" s="2">
         <v>0</v>
       </c>
-      <c r="EQ14" s="49"/>
+      <c r="EQ14" s="50"/>
       <c r="ER14" s="3">
         <f t="shared" si="1"/>
         <v>199</v>
@@ -5164,7 +5164,7 @@
       <c r="FE14" s="2">
         <v>0</v>
       </c>
-      <c r="FF14" s="49"/>
+      <c r="FF14" s="50"/>
       <c r="FG14" s="3">
         <f t="shared" si="7"/>
         <v>199</v>
@@ -5262,7 +5262,7 @@
       <c r="EP15" s="2">
         <v>3.2520325203252001E-2</v>
       </c>
-      <c r="EQ15" s="49"/>
+      <c r="EQ15" s="50"/>
       <c r="ER15" s="3">
         <f t="shared" si="1"/>
         <v>4562</v>
@@ -5304,7 +5304,7 @@
       <c r="FE15" s="2">
         <v>8.7680841736080695E-3</v>
       </c>
-      <c r="FF15" s="49"/>
+      <c r="FF15" s="50"/>
       <c r="FG15" s="3">
         <f t="shared" si="7"/>
         <v>4562</v>
@@ -5402,7 +5402,7 @@
       <c r="EP16" s="2">
         <v>8.9430894308943094E-3</v>
       </c>
-      <c r="EQ16" s="49"/>
+      <c r="EQ16" s="50"/>
       <c r="ER16" s="3">
         <f t="shared" si="1"/>
         <v>2480</v>
@@ -5444,7 +5444,7 @@
       <c r="FE16" s="2">
         <v>4.4354838709677403E-3</v>
       </c>
-      <c r="FF16" s="49"/>
+      <c r="FF16" s="50"/>
       <c r="FG16" s="3">
         <f t="shared" si="7"/>
         <v>2480</v>
@@ -5544,7 +5544,7 @@
       <c r="EP17" s="2">
         <v>0</v>
       </c>
-      <c r="EQ17" s="49"/>
+      <c r="EQ17" s="50"/>
       <c r="ER17" s="3">
         <f t="shared" si="1"/>
         <v>172</v>
@@ -5586,7 +5586,7 @@
       <c r="FE17" s="2">
         <v>0</v>
       </c>
-      <c r="FF17" s="49"/>
+      <c r="FF17" s="50"/>
       <c r="FG17" s="3">
         <f t="shared" si="7"/>
         <v>172</v>
@@ -5675,7 +5675,7 @@
       <c r="EP18" s="2">
         <v>9.7560975609756097E-3</v>
       </c>
-      <c r="EQ18" s="49"/>
+      <c r="EQ18" s="50"/>
       <c r="ER18" s="3">
         <f t="shared" si="1"/>
         <v>824</v>
@@ -5717,7 +5717,7 @@
       <c r="FE18" s="2">
         <v>1.45631067961165E-2</v>
       </c>
-      <c r="FF18" s="49"/>
+      <c r="FF18" s="50"/>
       <c r="FG18" s="3">
         <f t="shared" si="7"/>
         <v>824</v>
@@ -5814,7 +5814,7 @@
       <c r="EP19" s="2">
         <v>1.6260162601626001E-2</v>
       </c>
-      <c r="EQ19" s="49"/>
+      <c r="EQ19" s="50"/>
       <c r="ER19" s="3">
         <f t="shared" si="1"/>
         <v>1402</v>
@@ -5856,7 +5856,7 @@
       <c r="FE19" s="2">
         <v>1.4265335235378001E-2</v>
       </c>
-      <c r="FF19" s="49"/>
+      <c r="FF19" s="50"/>
       <c r="FG19" s="3">
         <f t="shared" si="7"/>
         <v>1402</v>
@@ -5909,7 +5909,7 @@
       <c r="EP20" s="2">
         <v>2.4390243902438998E-3</v>
       </c>
-      <c r="EQ20" s="49"/>
+      <c r="EQ20" s="50"/>
       <c r="ER20" s="3">
         <f t="shared" si="1"/>
         <v>2274</v>
@@ -5951,7 +5951,7 @@
       <c r="FE20" s="2">
         <v>1.31926121372032E-3</v>
       </c>
-      <c r="FF20" s="49"/>
+      <c r="FF20" s="50"/>
       <c r="FG20" s="3">
         <f t="shared" si="7"/>
         <v>2274</v>
@@ -6004,7 +6004,7 @@
       <c r="EP21" s="2">
         <v>0.141463414634146</v>
       </c>
-      <c r="EQ21" s="49"/>
+      <c r="EQ21" s="50"/>
       <c r="ER21" s="3">
         <f t="shared" si="1"/>
         <v>5622</v>
@@ -6046,7 +6046,7 @@
       <c r="FE21" s="2">
         <v>3.0949839914621101E-2</v>
       </c>
-      <c r="FF21" s="49"/>
+      <c r="FF21" s="50"/>
       <c r="FG21" s="3">
         <f t="shared" si="7"/>
         <v>5622</v>
@@ -6099,7 +6099,7 @@
       <c r="EP22" s="2">
         <v>6.50406504065041E-3</v>
       </c>
-      <c r="EQ22" s="49"/>
+      <c r="EQ22" s="50"/>
       <c r="ER22" s="3">
         <f t="shared" si="1"/>
         <v>606</v>
@@ -6141,7 +6141,7 @@
       <c r="FE22" s="2">
         <v>1.32013201320132E-2</v>
       </c>
-      <c r="FF22" s="49"/>
+      <c r="FF22" s="50"/>
       <c r="FG22" s="3">
         <f t="shared" si="7"/>
         <v>606</v>
@@ -6194,7 +6194,7 @@
       <c r="EP23" s="2">
         <v>2.6829268292682899E-2</v>
       </c>
-      <c r="EQ23" s="49"/>
+      <c r="EQ23" s="50"/>
       <c r="ER23" s="3">
         <f t="shared" si="1"/>
         <v>943</v>
@@ -6236,7 +6236,7 @@
       <c r="FE23" s="2">
         <v>3.4994697773064701E-2</v>
       </c>
-      <c r="FF23" s="49"/>
+      <c r="FF23" s="50"/>
       <c r="FG23" s="3">
         <f t="shared" si="7"/>
         <v>943</v>
@@ -6289,7 +6289,7 @@
       <c r="EP24" s="2">
         <v>1.05691056910569E-2</v>
       </c>
-      <c r="EQ24" s="49"/>
+      <c r="EQ24" s="50"/>
       <c r="ER24" s="3">
         <f t="shared" si="1"/>
         <v>2141</v>
@@ -6331,7 +6331,7 @@
       <c r="FE24" s="2">
         <v>6.0719290051377897E-3</v>
       </c>
-      <c r="FF24" s="49"/>
+      <c r="FF24" s="50"/>
       <c r="FG24" s="3">
         <f t="shared" si="7"/>
         <v>2141</v>
@@ -6384,7 +6384,7 @@
       <c r="EP25" s="2">
         <v>3.2520325203252002E-3</v>
       </c>
-      <c r="EQ25" s="49"/>
+      <c r="EQ25" s="50"/>
       <c r="ER25" s="3">
         <f t="shared" si="1"/>
         <v>1438</v>
@@ -6426,7 +6426,7 @@
       <c r="FE25" s="2">
         <v>2.7816411682892901E-3</v>
       </c>
-      <c r="FF25" s="49"/>
+      <c r="FF25" s="50"/>
       <c r="FG25" s="3">
         <f t="shared" si="7"/>
         <v>1438</v>
@@ -6479,7 +6479,7 @@
       <c r="EP26" s="2">
         <v>1.3008130081300801E-2</v>
       </c>
-      <c r="EQ26" s="49"/>
+      <c r="EQ26" s="50"/>
       <c r="ER26" s="3">
         <f t="shared" si="1"/>
         <v>2572</v>
@@ -6521,7 +6521,7 @@
       <c r="FE26" s="2">
         <v>6.2208398133748099E-3</v>
       </c>
-      <c r="FF26" s="49"/>
+      <c r="FF26" s="50"/>
       <c r="FG26" s="3">
         <f t="shared" si="7"/>
         <v>2572</v>
@@ -6574,7 +6574,7 @@
       <c r="EP27" s="2">
         <v>9.7560975609756097E-3</v>
       </c>
-      <c r="EQ27" s="49"/>
+      <c r="EQ27" s="50"/>
       <c r="ER27" s="3">
         <f t="shared" si="1"/>
         <v>1472</v>
@@ -6616,7 +6616,7 @@
       <c r="FE27" s="2">
         <v>8.1521739130434798E-3</v>
       </c>
-      <c r="FF27" s="49"/>
+      <c r="FF27" s="50"/>
       <c r="FG27" s="3">
         <f t="shared" si="7"/>
         <v>1472</v>
@@ -6669,7 +6669,7 @@
       <c r="EP28" s="2">
         <v>0.18373983739837399</v>
       </c>
-      <c r="EQ28" s="49"/>
+      <c r="EQ28" s="50"/>
       <c r="ER28" s="3">
         <f t="shared" si="1"/>
         <v>2510</v>
@@ -6711,7 +6711,7 @@
       <c r="FE28" s="2">
         <v>9.00398406374502E-2</v>
       </c>
-      <c r="FF28" s="49"/>
+      <c r="FF28" s="50"/>
       <c r="FG28" s="3">
         <f t="shared" si="7"/>
         <v>2510</v>
@@ -6764,7 +6764,7 @@
       <c r="EP29" s="2">
         <v>5.3658536585365901E-2</v>
       </c>
-      <c r="EQ29" s="49"/>
+      <c r="EQ29" s="50"/>
       <c r="ER29" s="3">
         <f t="shared" si="1"/>
         <v>1958</v>
@@ -6806,7 +6806,7 @@
       <c r="FE29" s="2">
         <v>3.3707865168539297E-2</v>
       </c>
-      <c r="FF29" s="49"/>
+      <c r="FF29" s="50"/>
       <c r="FG29" s="3">
         <f t="shared" si="7"/>
         <v>1958</v>
@@ -6859,7 +6859,7 @@
       <c r="EP30" s="2">
         <v>6.50406504065041E-3</v>
       </c>
-      <c r="EQ30" s="49"/>
+      <c r="EQ30" s="50"/>
       <c r="ER30" s="3">
         <f t="shared" si="1"/>
         <v>1232</v>
@@ -6901,7 +6901,7 @@
       <c r="FE30" s="2">
         <v>6.4935064935064896E-3</v>
       </c>
-      <c r="FF30" s="49"/>
+      <c r="FF30" s="50"/>
       <c r="FG30" s="3">
         <f t="shared" si="7"/>
         <v>1232</v>
@@ -6954,7 +6954,7 @@
       <c r="EP31" s="2">
         <v>1.21951219512195E-2</v>
       </c>
-      <c r="EQ31" s="49"/>
+      <c r="EQ31" s="50"/>
       <c r="ER31" s="3">
         <f t="shared" si="1"/>
         <v>301</v>
@@ -6996,7 +6996,7 @@
       <c r="FE31" s="2">
         <v>4.9833887043189397E-2</v>
       </c>
-      <c r="FF31" s="49"/>
+      <c r="FF31" s="50"/>
       <c r="FG31" s="3">
         <f t="shared" si="7"/>
         <v>301</v>
@@ -7049,7 +7049,7 @@
       <c r="EP32" s="2">
         <v>3.2520325203252002E-3</v>
       </c>
-      <c r="EQ32" s="49"/>
+      <c r="EQ32" s="50"/>
       <c r="ER32" s="3">
         <f t="shared" si="1"/>
         <v>129</v>
@@ -7091,7 +7091,7 @@
       <c r="FE32" s="2">
         <v>3.1007751937984499E-2</v>
       </c>
-      <c r="FF32" s="49"/>
+      <c r="FF32" s="50"/>
       <c r="FG32" s="3">
         <f t="shared" si="7"/>
         <v>129</v>
@@ -7144,7 +7144,7 @@
       <c r="EP33" s="2">
         <v>0.104065040650407</v>
       </c>
-      <c r="EQ33" s="49"/>
+      <c r="EQ33" s="50"/>
       <c r="ER33" s="3">
         <f t="shared" si="1"/>
         <v>2370</v>
@@ -7186,7 +7186,7 @@
       <c r="FE33" s="2">
         <v>5.4008438818565402E-2</v>
       </c>
-      <c r="FF33" s="49"/>
+      <c r="FF33" s="50"/>
       <c r="FG33" s="3">
         <f t="shared" si="7"/>
         <v>2370</v>
@@ -7239,7 +7239,7 @@
       <c r="EP34" s="2">
         <v>0.16585365853658501</v>
       </c>
-      <c r="EQ34" s="49"/>
+      <c r="EQ34" s="50"/>
       <c r="ER34" s="3">
         <f t="shared" si="1"/>
         <v>1727</v>
@@ -7281,7 +7281,7 @@
       <c r="FE34" s="2">
         <v>0.11812391430225801</v>
       </c>
-      <c r="FF34" s="49"/>
+      <c r="FF34" s="50"/>
       <c r="FG34" s="3">
         <f t="shared" si="7"/>
         <v>1727</v>
@@ -7334,7 +7334,7 @@
       <c r="EP35" s="2">
         <v>1.6260162601626001E-3</v>
       </c>
-      <c r="EQ35" s="49"/>
+      <c r="EQ35" s="50"/>
       <c r="ER35" s="3">
         <f t="shared" si="1"/>
         <v>711</v>
@@ -7376,7 +7376,7 @@
       <c r="FE35" s="2">
         <v>2.81293952180028E-3</v>
       </c>
-      <c r="FF35" s="49"/>
+      <c r="FF35" s="50"/>
       <c r="FG35" s="3">
         <f t="shared" si="7"/>
         <v>711</v>
@@ -7429,7 +7429,7 @@
       <c r="EP36" s="2">
         <v>0.18292682926829301</v>
       </c>
-      <c r="EQ36" s="49"/>
+      <c r="EQ36" s="50"/>
       <c r="ER36" s="3">
         <f t="shared" si="1"/>
         <v>4970</v>
@@ -7471,7 +7471,7 @@
       <c r="FE36" s="2">
         <v>4.5271629778672003E-2</v>
       </c>
-      <c r="FF36" s="49"/>
+      <c r="FF36" s="50"/>
       <c r="FG36" s="3">
         <f t="shared" si="7"/>
         <v>4970</v>
@@ -7524,7 +7524,7 @@
       <c r="EP37" s="24">
         <v>2.4390243902438998E-3</v>
       </c>
-      <c r="EQ37" s="50"/>
+      <c r="EQ37" s="51"/>
       <c r="ER37" s="3">
         <f t="shared" si="1"/>
         <v>444</v>
@@ -7566,7 +7566,7 @@
       <c r="FE37" s="24">
         <v>6.7567567567567597E-3</v>
       </c>
-      <c r="FF37" s="50"/>
+      <c r="FF37" s="51"/>
       <c r="FG37" s="3">
         <f t="shared" si="7"/>
         <v>444</v>
@@ -7942,6 +7942,75 @@
     </row>
   </sheetData>
   <mergeCells count="85">
+    <mergeCell ref="FF5:FF9"/>
+    <mergeCell ref="FF11:FF37"/>
+    <mergeCell ref="EU1:FH2"/>
+    <mergeCell ref="EU3:EU4"/>
+    <mergeCell ref="EV3:EW3"/>
+    <mergeCell ref="EX3:EY3"/>
+    <mergeCell ref="EZ3:FA3"/>
+    <mergeCell ref="FB3:FC3"/>
+    <mergeCell ref="FD3:FE3"/>
+    <mergeCell ref="FF3:FF4"/>
+    <mergeCell ref="FG3:FH3"/>
+    <mergeCell ref="BB5:BB9"/>
+    <mergeCell ref="CV1:CX2"/>
+    <mergeCell ref="BX1:BZ2"/>
+    <mergeCell ref="CF1:CH2"/>
+    <mergeCell ref="CB1:CD2"/>
+    <mergeCell ref="CN1:CP2"/>
+    <mergeCell ref="CJ1:CL2"/>
+    <mergeCell ref="BR3:BS3"/>
+    <mergeCell ref="AB1:AD2"/>
+    <mergeCell ref="B5:B9"/>
+    <mergeCell ref="T5:T9"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="B1:U2"/>
+    <mergeCell ref="X1:Z2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="T3:T4"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="U3:U4"/>
+    <mergeCell ref="BH3:BI3"/>
+    <mergeCell ref="CZ1:DB2"/>
+    <mergeCell ref="DD1:DF2"/>
+    <mergeCell ref="DH1:DJ2"/>
+    <mergeCell ref="AT3:AU3"/>
+    <mergeCell ref="AV3:AW3"/>
+    <mergeCell ref="AX3:AX4"/>
+    <mergeCell ref="AY3:AY4"/>
+    <mergeCell ref="BJ3:BK3"/>
+    <mergeCell ref="BL3:BM3"/>
+    <mergeCell ref="BT3:BT4"/>
+    <mergeCell ref="BU3:BU4"/>
+    <mergeCell ref="BF3:BG3"/>
+    <mergeCell ref="AL3:AM3"/>
+    <mergeCell ref="AN3:AO3"/>
+    <mergeCell ref="AF3:AG4"/>
+    <mergeCell ref="AH3:AI3"/>
+    <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="EM3:EN3"/>
+    <mergeCell ref="EO3:EP3"/>
+    <mergeCell ref="DL1:DN2"/>
+    <mergeCell ref="DP1:DR2"/>
+    <mergeCell ref="AF5:AF9"/>
+    <mergeCell ref="BN3:BO3"/>
+    <mergeCell ref="BP3:BQ3"/>
+    <mergeCell ref="BT5:BT9"/>
+    <mergeCell ref="AF1:AY2"/>
+    <mergeCell ref="CR1:CT2"/>
+    <mergeCell ref="AP3:AQ3"/>
+    <mergeCell ref="AR3:AS3"/>
+    <mergeCell ref="AX5:AX9"/>
+    <mergeCell ref="BB1:BU2"/>
+    <mergeCell ref="BB3:BC4"/>
+    <mergeCell ref="BD3:BE3"/>
     <mergeCell ref="DD11:DF12"/>
     <mergeCell ref="ER3:ES3"/>
     <mergeCell ref="EF1:ES2"/>
@@ -7958,75 +8027,6 @@
     <mergeCell ref="EG3:EH3"/>
     <mergeCell ref="EI3:EJ3"/>
     <mergeCell ref="EK3:EL3"/>
-    <mergeCell ref="EM3:EN3"/>
-    <mergeCell ref="EO3:EP3"/>
-    <mergeCell ref="DL1:DN2"/>
-    <mergeCell ref="DP1:DR2"/>
-    <mergeCell ref="AF5:AF9"/>
-    <mergeCell ref="BN3:BO3"/>
-    <mergeCell ref="BP3:BQ3"/>
-    <mergeCell ref="BT5:BT9"/>
-    <mergeCell ref="AF1:AY2"/>
-    <mergeCell ref="CR1:CT2"/>
-    <mergeCell ref="AP3:AQ3"/>
-    <mergeCell ref="AR3:AS3"/>
-    <mergeCell ref="AX5:AX9"/>
-    <mergeCell ref="BB1:BU2"/>
-    <mergeCell ref="BB3:BC4"/>
-    <mergeCell ref="BD3:BE3"/>
-    <mergeCell ref="BF3:BG3"/>
-    <mergeCell ref="AL3:AM3"/>
-    <mergeCell ref="AN3:AO3"/>
-    <mergeCell ref="AF3:AG4"/>
-    <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="BH3:BI3"/>
-    <mergeCell ref="CZ1:DB2"/>
-    <mergeCell ref="DD1:DF2"/>
-    <mergeCell ref="DH1:DJ2"/>
-    <mergeCell ref="AT3:AU3"/>
-    <mergeCell ref="AV3:AW3"/>
-    <mergeCell ref="AX3:AX4"/>
-    <mergeCell ref="AY3:AY4"/>
-    <mergeCell ref="BJ3:BK3"/>
-    <mergeCell ref="BL3:BM3"/>
-    <mergeCell ref="AJ3:AK3"/>
-    <mergeCell ref="B1:U2"/>
-    <mergeCell ref="X1:Z2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="T3:T4"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="U3:U4"/>
-    <mergeCell ref="AB1:AD2"/>
-    <mergeCell ref="B5:B9"/>
-    <mergeCell ref="T5:T9"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="R3:S3"/>
-    <mergeCell ref="BT3:BT4"/>
-    <mergeCell ref="BU3:BU4"/>
-    <mergeCell ref="BB5:BB9"/>
-    <mergeCell ref="CV1:CX2"/>
-    <mergeCell ref="BX1:BZ2"/>
-    <mergeCell ref="CF1:CH2"/>
-    <mergeCell ref="CB1:CD2"/>
-    <mergeCell ref="CN1:CP2"/>
-    <mergeCell ref="CJ1:CL2"/>
-    <mergeCell ref="BR3:BS3"/>
-    <mergeCell ref="FF5:FF9"/>
-    <mergeCell ref="FF11:FF37"/>
-    <mergeCell ref="EU1:FH2"/>
-    <mergeCell ref="EU3:EU4"/>
-    <mergeCell ref="EV3:EW3"/>
-    <mergeCell ref="EX3:EY3"/>
-    <mergeCell ref="EZ3:FA3"/>
-    <mergeCell ref="FB3:FC3"/>
-    <mergeCell ref="FD3:FE3"/>
-    <mergeCell ref="FF3:FF4"/>
-    <mergeCell ref="FG3:FH3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>